<commit_message>
Added cookies logic to avoid insta block
</commit_message>
<xml_diff>
--- a/instagram/data.xlsx
+++ b/instagram/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,6 +815,69 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>The reel features a mix of emotional and romantic content with high engagement, indicating a strong connection with the audience.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Romantic and emotional content creator with a focus on love and relationships.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Positive and engaging, with a lot of love and emotional reactions.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>18500</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reels/DIbGiMcxUvJ/</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/_pihu_arya2425/</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>The reel has high engagement and a romantic theme, which aligns well with Knytt's focus on personal connections. The creator's audience is likely to be interested in a texting &amp; video calling app.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Hey Pihu! Loved your reel—such a beautiful expression of love! 💖 We’re building Knytt, a cozy space for heartfelt conversations. Would love for you to check it out and maybe share your thoughts with your audience. Let’s connect! 😊</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>This is so heartfelt! 💖 If you ever want to share more love stories, Knytt is perfect for deep, personal convos. Check it out! 😊</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added model config roation
</commit_message>
<xml_diff>
--- a/instagram/data.xlsx
+++ b/instagram/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3902,6 +3902,69 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>A reel showcasing Delhi University’s famous Paneer Singapore Chowmein, priced at 180/-, located at Nams Momos, Kamla Nagar, Delhi. The content focuses on food and local Delhi culture, with high engagement from an Indian audience.</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Food enthusiast and local Delhi explorer, likely a student or young adult, creating relatable food content for a Delhi-based audience.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Casual and appreciative, focusing on the food and local vibe.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>7</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DL4bFQiyOhX/</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/yumm_hmm__</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>The creator focuses on Delhi-specific food content, indicating a strong Indian audience, which aligns with Knytt's target market. The reel has positive engagement (emojis like 😍, 🔥, ❤️), suggesting an active and interested audience. While the creator may be interested in joining a platform like Knytt to connect with foodies, the likelihood is medium due to the niche focus on food rather than personal interaction. A comment can engage the audience, while a personalized DM can directly pitch to the creator.</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Hey @yumm_hmm__, loved your reel on Paneer Singapore Chowmein! 😍 We’re building a cool app called Knytt where foodies like you can connect with fans through texting and video calls. Would love to have you on board to share your Delhi food adventures! Check us out at knytt.in or drop me a message if you’re curious. ✨</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>This looks insanely delicious! 😍 Kamla Nagar always has the best eats. If you’re a foodie, you’d love connecting with more peeps on @knyttofficial! 🍝🔥</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added login session incognito
</commit_message>
<xml_diff>
--- a/instagram/data.xlsx
+++ b/instagram/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4403,6 +4403,1500 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>A serene and poetic reel showcasing quiet, heartfelt moments from Uttarakhand's mountains, evoking nostalgia and appreciation for nature's beauty and slow travel. The audience responds with affectionate and emotional comments, indicating a strong connection to the content.</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>A thoughtful, nature-loving creator focused on mindful travel and cultural appreciation, resonating deeply with an audience that values emotional and scenic storytelling from India, especially Uttarakhand.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Highly positive, emotional, nostalgic, and appreciative.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>8</v>
+      </c>
+      <c r="G64" t="n">
+        <v>30</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMh5G0zICU2/</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/thepahadistory</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>The reel’s emotional richness and cultural specificity aligns well with Knytt’s focus on authentic, personal connections and Indian users. The creator’s niche and engaged audience make them a strong candidate for conversion. Commenting on the reel would engage the audience in an organic way, while a personalized DM to the creator could invite collaboration on Knytt, emphasizing shared values of meaningful connections and storytelling.</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Hi there! Your beautiful reel perfectly captures the soulful essence of Uttarakhand and those quiet, meaningful moments we all cherish. At Knytt, we’re building a space where creators like you can connect deeply with fans via texting and video calls — sharing stories and memories just like yours. We’d love to have you on board to bring more heartfelt Indian stories to life. Interested in chatting? 😊",
+  "public_comment": "Such peaceful vibes and beautiful memories in every frame! Your reel truly warms the heart, just like a good cup of chai ☕️✨. Creators like you would be amazing on platforms like Knytt, where authentic stories and connections blossom. Keep shining! 🌿❤️ #IncredibleIndia"</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>The reel showcases relatable, emotional content that resonates well with the Indian audience, reflected in the high engagement and supportive comments. The creator appears to be an Indian content creator focusing on everyday life and emotional storytelling. The audience tone is warm, positive, and engaged, often sharing personal experiences in the comments. The reel has a substantial number of likes, indicating good reach and viral potential.</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Indian emotional storyteller with a strong connection to their followers, focusing on relatable and heartfelt content that promotes engagement and community.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Positive and supportive with a strong emotional connection.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>8</v>
+      </c>
+      <c r="G65" t="n">
+        <v>12000</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMFLLszR1rw/</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorprofile</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>The creator's content is highly relatable and emotionally engaging, which fits well with Knytt's focus on personal connection via texting and video calls. The high engagement and positive sentiment suggest the creator is likely to be interested in joining a platform that enhances personal communication. A personalized DM can encourage them to join, while a comment can spark curiosity among their audience.</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Hi! Loved how your reel beautifully captures real emotions—it's exactly the kind of genuine connection we value at Knytt. We're building a fun, safe space for texting and video calls across India and would love to have you join our creator community to connect even deeper with your followers. Interested in exploring? 😊</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>Your reel really hits home! ❤️ If you and your amazing audience love deep, real conversations, you might enjoy checking out Knytt – a cool new app for texting &amp; video calls, made just for India! #StayConnected</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>The reel is a heartfelt share about personal growth and overcoming challenges, resonating deeply with viewers who appreciate genuine and emotional content. The creator appears to be an Indian individual focused on motivational and relatable themes, engaging a supportive audience that values meaningful connections.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Motivational and relatable content creator with a strong emotional connection to their audience, primarily Indian youth seeking inspiration and authentic interactions.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Supportive and empathetic, with many viewers expressing encouragement and personal identification with the message.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>8</v>
+      </c>
+      <c r="G66" t="n">
+        <v>12000</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMc1-iAOgxc/</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creator_handle</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>The creator's content aligns well with Knytt's focus on personal, direct communication through texting and video calls. Given the emotional depth and Indian audience, this creator is likely to convert and can also help engage their followers. Commenting will foster audience interaction, while a personalized DM can invite the creator to expand their engagement on Knytt.</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Hi! Loved how your reel touches hearts and inspires real connections. Knytt is a new app designed for meaningful, personal chats and video calls—perfect for creators like you who value genuine engagement. Would love to have you join and connect with your fans even more closely. Interested in giving it a try?</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>This really hits home! Love how you keep it so real and inspiring. If anyone’s looking for a space to connect deeper, you should check out Knytt—it’s where real conversations happen!</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>The reel features a relatable and heartfelt moment about daily struggles and perseverance, resonating well with an Indian audience. The creator shares personal stories that connect emotionally, attracting a warm and engaged community.</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>An emotionally expressive, motivational content creator with a strong connection to Indian youth and working professionals, focusing on real-life challenges and positivity.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Positive, empathetic, and supportive</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>8</v>
+      </c>
+      <c r="G67" t="n">
+        <v>12500</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMftq6sKsjh/</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorhandle</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>The creator's content is emotionally rich and relatable, making a comment beneficial to engage the audience and boost reach. The creator’s persona and engagement levels indicate a strong likelihood of conversion via a personalized DM that highlights how Knytt can deepen their audience connection through personal texting and video calling.</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Hi! Loved how genuinely your reel captured everyday struggles and motivation — it really resonates. We think you’d be a perfect fit for Knytt, a new app where you can connect with your fans directly through texting and video calls, creating deeper, more personal engagement. Would love to chat more if you’re interested!</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>This really hits home! 💯 Sometimes we all need that little extra connection — if you’re curious about more ways to keep the conversation going with your fans, check out Knytt! 😊</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>The reel features a relatable and emotional theme about personal growth and self-acceptance, resonating well with a primarily young Indian audience. The creator shares authentic content that engages viewers deeply, as reflected by the warm and supportive comments. The reel has a moderate number of likes, indicating decent reach and potential for further engagement.</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>A young Indian content creator focused on mental wellness, self-improvement, and authentic storytelling. They connect deeply with their audience through vulnerability and motivational content.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Supportive, empathetic, and encouraging with viewers relating personally to the message.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>8</v>
+      </c>
+      <c r="G68" t="n">
+        <v>12000</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMh1Ct7oB6T/</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorhandle</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>The creator's content aligns well with Knytt’s focus on personal connection and meaningful communication. The emotional and authentic tone of the reel suggests the creator's audience is engaged and open to intimate, paid texting and video calling experiences. Both a personalized DM and a supportive, contextually relevant comment would maximize engagement and conversion potential.</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Hey! Loved your recent reel about self-growth and authenticity — it really struck a chord with me. I think your audience would really vibe with Knytt, a new app for paid texting and video calls that helps creators connect deeply with fans in India. Would love to chat about how we can collaborate and bring more meaningful conversations to your community!</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>This reel hits so deep! 🌟 It’s amazing to see such honest and uplifting content. If you're looking to connect even more personally with your community, you might want to check out @knyttofficial — it's a cool new app for real, meaningful chats!</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>The reel features a popular Indian content creator known for relatable and humorous takes on everyday life, especially focusing on family and social situations. The content has garnered significant engagement with a high number of likes and views, indicating strong audience resonance. The creator's style is casual and comedic, appealing primarily to young Indian adults who enjoy light-hearted, culturally relevant content.</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Young Indian content creator specializing in relatable, comedic reels about daily life and social/family scenarios, with a warm and engaging style.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Positive and enthusiastic, with audience reactions including laughter, tagging friends, and sharing personal anecdotes that align with the reel's theme.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>8</v>
+      </c>
+      <c r="G69" t="n">
+        <v>25000</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMkgO6zpSvP/</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/examplecreator/</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>The creator's content strongly aligns with Knytt's focus on personal connections via texting and video calls. The high engagement and culturally relevant humor make the creator an excellent candidate for partnership. Commenting will engage the audience organically, while a personalized DM can establish a direct connection with the creator to discuss collaboration opportunities.</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Hey! Loved your recent reel — your content really captures the fun and warmth of everyday Indian life. I’m reaching out from Knytt, a new Indian app for paid texting and video calls that helps creators build closer connections with their fans. We think you’d be a perfect fit and would love to chat about how we can support you and your community. Interested in learning more?</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>Totally vibing with this! If you love connecting with fans as much as we do, you should check out @knyttofficial — it’s all about bringing creators and fans closer with texting &amp; video calls. 🔥</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Priya P Varrier posted a heartfelt reel captioned 'For the feeling you never had words for.💛 #JhimJhim says it for you!✨' promoting a full song on a YouTube channel. The reel has a warm, emotional tone with many fans leaving loving and supportive comments filled with hearts and fire emojis, showing strong positive engagement.</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Priya P Varrier is an emotionally expressive and popular Indian creator associated with music and entertainment content, appealing to a young, affectionate audience.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Highly positive and affectionate, with followers expressing love, admiration, and warmth.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>8</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DLZKpTTxhq5/</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/priya.p.varrier</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>The creator's content is emotionally rich and relatable, with an engaged Indian audience that resonates well with heartfelt messaging. Priya's popularity and the affectionate comments indicate a strong potential for conversion to Knytt, which benefits from personal, emotional connection. Outreach via both a personalized DM to Priya and a public comment would maximize reach and engagement.</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Hi Priya! Your reel beautifully captures those feelings words can't express — it really struck a chord! We think your vibe would be perfect for Knytt, a new Indian app where you can connect deeply with fans via texting and video calls. It’s a great way to share those special moments directly with your audience. Would love to have you onboard and see you shine there!</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>This reel hits right in the feels! 💛 Priya, your fans would love connecting with you even more on Knytt — a fresh app just for India where you can chat and video call your biggest supporters! 🚀</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>The reel features a humorous and relatable take on everyday struggles, resonating well with a young Indian audience. The creator uses simple, candid storytelling to engage viewers, which has earned a moderate number of likes and positive, lighthearted comments.</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>A young, relatable Indian content creator who shares everyday life humor and relatable moments with their audience, primarily targeting Indian youth.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Positive and humorous, with engagement reflecting amusement and relatability.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>8</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMdJAw-oYPp/</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/examplecreator</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>The creator’s content style aligns well with Knytt’s casual and personal communication platform, and their audience matches the Indian user base Knytt is targeting. The engagement is positive, indicating openness to new interactive experiences. Both DM and comment outreach will help attract attention from both creator and audience.</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Hey! Loved your reel—your humor and relatable vibe really stand out. We think you'd be a perfect fit for Knytt, a new Indian-only texting &amp; video calling app that connects creators directly with their community in a fun, personal way. Would love to have you join and share your unique style with our users! Interested in learning more?</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>This reel just made my day! If you love connecting with your fans as much as you nail these moments, have you checked out Knytt? It’s a cool Indian app where creators and fans can chat and video call easily. Worth a look! 😊</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>This reel features Annie, a beloved cat who has found a forever home along with her kittens. The audience expresses a warm, affectionate tone with numerous heart emojis and compliments highlighting Annie's cuteness and the touching story of adoption. Comments show emotional engagement, particularly from pet lovers who resonate with the adoption theme.</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Animal lover and pet advocate, likely focused on adoption and care for cats, with a compassionate and heartfelt approach to sharing pet stories.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Highly positive, affectionate, empathetic, and supportive.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>7</v>
+      </c>
+      <c r="G72" t="n">
+        <v>13</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMfV2Q0uD0Q/</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bethostern</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>The creator's focus on animal welfare and the emotional, relatable content about pet adoption fits well with Knytt's value of personal, meaningful connections. The affectionate and engaged audience also presents an opportunity to extend reach. The reel's moderate likes suggest some viral potential but more niche appeal.</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Hi Beth! I love how you share Annie’s heartwarming story and the love around pet adoption—it really connects with people on a personal level. We think creators like you would truly shine on Knytt, our app for genuine video calls and texting that help build real, caring communities. Would love to have you join and bring your amazing vibe to Knytt! Check it out here: https://knytt.in</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Annie and her nuggets are just too precious! 🐾❤️ Love seeing such sweet stories of forever homes. You’ve got a really lovely community here! If you’re ever curious about new ways to connect with your fans, check out @knyttofficial—it's all about real, heartfelt connections. 😊</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>The reel showcases a heartfelt moment relatable to many Indian youth, capturing emotions around friendship and personal growth. The creator's content resonates emotionally with their audience, evidenced by high engagement and supportive comments.</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Young Indian content creator focusing on emotional and relatable life moments, connecting deeply with their audience through authentic storytelling.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Positive, empathetic, and supportive</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>8</v>
+      </c>
+      <c r="G73" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DL-D4yeRTe3/</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorusername/</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>The reel's emotional authenticity and strong audience engagement indicate the creator's openness to meaningful interaction, making them a great candidate for Knytt. A personal DM can introduce the platform tailored to their content style, while a comment can engage their audience naturally.</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Hey! Loved how you captured such real emotions in your reel—it really hits home. We have a new app called Knytt where creators like you can connect with fans through personal texting and video calls, creating even deeper bonds. Would love to explore if you'd be interested in joining this growing community in India!</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>This reel truly speaks to the soul! For anyone wanting to dive deeper into genuine connections like these, check out @knyttofficial—it’s a cool new way to stay close with creators you vibe with!</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>The reel beautifully showcases monsoon vibes in Kerala, specifically around Palakkad and Thrissur, encouraging viewers to enjoy the monsoon with friends. The creator tags local spots and friends, creating a warm, communal feeling. The audience responds with overwhelmingly positive, affectionate emojis like hearts and fire, showing emotional resonance and local pride.</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>A local content creator passionate about Kerala's natural beauty and monsoon season, with a friendly and community-oriented style.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Highly positive, affectionate, and nostalgic</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>7</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DKMlQ4uxTzD/</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ayem.aswin</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>The creator's content is emotionally rich and regionally relevant, resonating strongly with an Indian audience. The monsoon theme and local tagging make it natural to connect Knytt's app, which supports personal communication and sharing experiences, especially around close-knit moments like monsoons with friends. The lack of visible likes suggests moderate reach but strong engagement from a niche audience. Both a DM and a comment would help initiate personal connection and audience curiosity.</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Hey! Loved your reel capturing the magic of Kerala's monsoon — it really brings out those special moments with friends. Since you create such warm, local content, I think you'd vibe with Knytt, a new app where you can connect through texting and video calls with your close ones, all within India. Would love to have you join and share your monsoon stories there! Check it out if you're curious :)</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>This monsoon vibe is everything! 🌧️💚 Perfect reminder to cherish the moments with our loved ones. Have you heard of @knyttofficial? It's a cool new way to stay connected with your homies through texting and video calls—totally India-focused and just right for sharing monsoon feels!</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Chad Torkelsen shares a reflective reel with clips from popular shows, resonating emotionally with his audience who respond with encouragement and affection. The content is relatable and introspective, making it a good fit for engaging users who appreciate deep, meaningful content.</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Thoughtful, introspective storyteller with an interest in impactful media and emotional connection.</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Positive, supportive, and heartfelt</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>7</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMbRkP6hwcJ/</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/chadtorkelsen</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>The creator’s content is emotionally rich and relatable, which can engage the audience well through comments to spark curiosity. Chad’s thoughtful persona suggests he could appreciate a personal DM introducing Knytt as a platform for deeper, authentic connections. Audience engagement is supportive but not overly viral, so combining both outreach methods maximizes impact.</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Hey Chad, love how your reel captures life’s complex puzzle so thoughtfully! At Knytt, we’re building a space where real, meaningful conversations happen via texting and video calls — would be great to have someone with your vibe join us and inspire deeper connections. Would you be interested in checking it out?</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>This reel really hits deep — life’s puzzles are easier to face when we connect with others. If you’re into real chats and authentic bonds, you might want to check out @knyttofficial for some next-level connection vibes!</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Stianmklo shares a visually stunning and artistically rich infrared photography series from Greenland, capturing surreal and hauntingly beautiful images of icebergs. The audience, mainly photography enthusiasts, responds with admiration and praise for the textures, mood, and technique.</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>A passionate and skilled landscape and infrared photographer focused on artistic expression and capturing unique natural beauty through innovative techniques.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Highly positive and appreciative, with audience expressing admiration for the creativity and technical mastery.</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>7</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMnesDeo5b6/</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/stianmklo</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>The creator is highly artistic and technically skilled, which aligns well with Knytt's appeal to creators who want to connect deeply with their audience via personal texting and video calls. Although the reel lacks view and like metrics here, the quality of engagement is strong. A personalized DM can invite him to explore Knytt as a platform to share more personal stories behind his artistic process and build a closer fan community. Comments are less effective here since the reel is visually focused and the audience is niche and professional.</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>message</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Hi Stian, your infrared Greenland series is truly mesmerizing — it reveals an incredible hidden beauty in nature! We'd love to invite you to Knytt, a new Indian app where creators like you can connect directly with their fans through texting and video calls, sharing stories beyond posts. It's a great way to deepen your audience bond and explore new creative conversations. Would you be interested in checking it out? Here's the link: https://knytt.in",
+  "public_comment": null</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>The reel showcases the Ajanta Buddhist caves in Maharashtra, highlighting their historical and cultural significance with detailed descriptions and relevant hashtags. The audience responds with respectful and appreciative comments, mostly in Hindi and Marathi, expressing reverence for Buddha and pride in Indian heritage, with many using religious salutations like 'Namo Buddhay' and references to social reformers like Dr. Ambedkar and Jyotiba Phule.</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>A culturally rooted and informative creator focusing on Indian heritage, spirituality, and historical monuments, attracting an audience interested in Indian culture, history, and Buddhist philosophy.</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Positive, respectful, and reverential with a strong emotional connection to Indian culture and Buddhism.</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>7</v>
+      </c>
+      <c r="G77" t="n">
+        <v>16</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DJ0b_rLoTzE/</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/hisdhamma</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>The reel has moderate engagement but a highly engaged and culturally connected audience. The creator’s focus on Indian heritage and spirituality aligns well with Knytt’s Indian user base. The respectful and emotional tone of comments suggests that a thoughtful, culturally sensitive outreach could resonate well. Both a personalized DM to the creator and a public comment to engage the audience would be beneficial to grow curiosity around Knytt.</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Hi! Loved your beautiful reel on the Ajanta caves and the deep cultural pride you share. We think your followers, who appreciate India's rich heritage and meaningful connections, would really enjoy Knytt — a new app where you can chat and video call with like-minded people across India, keeping cultural conversations alive in a fun way! Would love to collaborate and bring your inspiring content to our community. Let me know if you'd be interested! 🙏✨",
+  "public_comment": "Absolutely loved this glimpse into the Ajanta caves! For everyone who treasures our heritage and meaningful connections, check out @knyttofficial — an app to chat and video call with fellow culture lovers across India! 🧡 #IncredibleIndia #StayConnected"</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>This reel features a highly addictive and calming song paired with a beautifully edited video that resonates emotionally with the audience. The comments are overwhelmingly positive, filled with heart and tear emojis reflecting deep emotional connection and appreciation for both the song and the edit.</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Creative music lover and editor who shares emotionally rich, calming content that deeply connects with their followers.</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Highly positive, emotional, and appreciative.</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>7</v>
+      </c>
+      <c r="G78" t="n">
+        <v>12</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DKRxvxjIKYU/</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/iadoreskiess</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>The creator shares emotionally engaging content with a small but engaged audience. The comments show an emotional connection that can be leveraged to encourage curiosity about Knytt as a platform for personal, heartfelt communication. The reel's reach is modest but the content quality and audience engagement are strong, justifying both a personalized DM and a casual, contextually relevant comment to maximize impact.</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Hey! Loved your reel—such a soothing vibe with that addictive song and your edit is truly on point. We have a cool app called Knytt that's all about connecting people through personal texting and video calls, and we think creators like you, who share emotional, relatable content, would really vibe with it. Would love to chat more if you're interested in exploring something new and meaningful for your followers!</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>This edit + song combo is pure magic! 🥹❤️ Your vibe totally fits the kind of heartfelt connections we celebrate on @knyttofficial. Would love to see you there sometime!</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>The reel showcases a beautiful travel video of Dhanushkodi, Tamil Nadu, capturing scenic drone footage. The audience response is overwhelmingly positive and emotive, with many expressing admiration and awe through heart and clap emojis. The creator appeals to travel lovers and those interested in Indian scenic spots.</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Travel enthusiast focused on exploring and showcasing serene Indian locations, particularly in Tamil Nadu, with a visually appealing and artistic style.</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Highly positive and appreciative, with emotional and admiring reactions from the audience.</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>7</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DLtS5vOzVhL/</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/charly.kc</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>The creator has a focused Indian travel niche which aligns well with Knytt's Indian user base. The emotionally rich and positive comments indicate a receptive audience. While direct likes count is not provided, the engagement in comments is strong, suggesting good reach. Both DM and comment outreach can be effective: DM for the creator to join and promote Knytt, and comment to spark curiosity among the audience.</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Hi Charly! Loved your breathtaking Dhanushkodi reel — your travel stories really capture the heart of India beautifully. We’d love to invite you to join Knytt, an exciting new Indian app for paid texting &amp; video calling that connects creators directly with their fans. It’s a great way to deepen connections with your audience and share your travel experiences more personally. Let me know if you’d be interested to know more!</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>Absolutely stunning views of Dhanushkodi! 😍 If you love connecting deeper with travel fans, check out @knyttofficial — a cool Indian app for chats and video calls that’s perfect for creators like you!</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>The creator Priyankha_bs_ shares energetic and confident content blending on-stage and off-stage vibes with music and dance elements. The reel uses popular Tamil and Indian cultural tags, suggesting a local Indian audience. The comments show enthusiastic, warm reactions with many fire and heart emojis, indicating a positive and engaged audience. The creator appears to have a vibrant persona appealing to music and dance fans, likely from South India.</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Energetic, confident performer with a strong connection to Tamil and Indian cultural music and dance, appealing to a young, passionate Indian audience.</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Very positive and enthusiastic, with many users expressing admiration and excitement.</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>7</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DLHphp_BDIa/</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/priyankha_bs_/</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>The creator’s content and audience are well aligned with Knytt’s India-focused app. The emotional and cultural connection in the reel suggests audience engagement that can be tapped via comments to spark curiosity. The creator’s confident and engaging style makes a personalized DM appealing to invite them to join Knytt and grow their reach.</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Hi Priyankha! Love how you slay on and off stage—your energy really shines through your reels. We think your vibe would be perfect for Knytt, a cool Indian app for paid texting &amp; video calls that helps creators connect deeply with their fans. Would love to have you onboard and help your amazing audience engage with you even more personally! Check it out here: https://knytt.in 😊",
+  "public_comment": "🔥 Your energy is infectious! Your fans would love connecting with you even more—have you heard of Knytt? It’s an awesome Indian app for paid texting &amp; video calls that lets creators build closer bonds with their audience. Worth a peek! 💥 #KnyttVibes"</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>The reel showcases a relatable and emotional moment that resonates well with the Indian audience, reflected in its high like count and engaging comments. The creator likely has a strong connection with their followers, making them an excellent candidate for personalized outreach to promote Knytt's unique texting and video calling features tailored for the Indian market.</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Engaged Indian content creator focusing on emotionally rich, relatable content that connects deeply with their audience.</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Positive, empathetic, and engaging with a touch of humor and warmth.</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>8</v>
+      </c>
+      <c r="G81" t="n">
+        <v>15200</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DBT2SuGPlHr/</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorprofile/</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>The reel's emotional depth and high engagement indicate a creator who can influence their audience effectively. Commenting can boost public engagement further, while a personalized DM can encourage direct collaboration. Their audience is primarily Indian, aligning perfectly with Knytt's current market.</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Hi! Loved your recent reel — it really struck a chord! We’re working on Knytt, a cool new texting and video calling app designed just for Indian creators and their fans to connect more personally. Would love to explore how you can bring that closer connection to your amazing community. Interested in chatting more?</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>This reel hits right in the feels! Imagine connecting even closer with your fans through a new app made just for Indian creators like you — check out @knyttofficial for something special!</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>The reel showcases scenic views of Alappuzha, Kerala, featuring drone shots and railway visuals. The audience reactions are overwhelmingly positive with many expressing admiration using heart and fire emojis. The creator uses location and thematic hashtags relevant to Kerala travel and drone videography.</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>A travel and nature enthusiast focused on Kerala, using drone videography to showcase beautiful landscapes and railway scenes, appealing to viewers who appreciate regional beauty and exploration.</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Highly positive, with viewers responding emotionally through emojis like hearts, fire, and expressions of awe, indicating strong visual appeal and emotional connection.</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>7</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DKyAqI7zUMc/</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/charly.kc</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>The creator’s content is visually engaging and regionally relevant to Indian audiences, particularly Kerala locals and enthusiasts, making them a good candidate for Knytt's app which targets Indian users interested in connection and sharing. The positive emotional response suggests that a comment could boost engagement and a DM could personalize the pitch inviting them to join Knytt to connect with their audience in a new way.</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Hi Charly! Your stunning drone shots of Alappuzha beautifully capture Kerala’s charm. We think your content would be a perfect fit for Knytt — a new app for paid texting &amp; video calls that helps creators connect more deeply with fans across India. Would love to explore how we can collaborate and help you grow your community!</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>Absolutely love these breathtaking views of Alappuzha! 😍 Kerala looks magical through your lens. Have you heard about Knytt? It’s a cool new app connecting creators and fans through chat and video calls — right here in India! Might be a great way to share more of your amazing journeys. 🚀</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>The reel showcases a serene reflection on spending time alone in nature to find peace and calmness. The caption is poetic and emotionally rich, emphasizing the importance of disconnecting from noise and pressure to reset one's mind. The audience's comments are overwhelmingly positive and appreciative, using heart and nature-related emojis, expressing admiration and agreement with the sentiment.</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>A thoughtful, nature-loving individual who values mindfulness and peaceful moments, likely attracting a calm and reflective audience interested in wellness and mental clarity.</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Positive, peaceful, and appreciative</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>7</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DJmZtJ3M9-x/</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/johandburan</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>The reel's emotionally rich and relatable content about mindfulness and nature makes it suitable for a comment to boost engagement and curiosity. The creator's persona aligns well with promoting a platform like Knytt that enables personal connections through texting and video calling, which can be positioned as a way to share peaceful moments or stay connected meaningfully. Hence, both comment and personalized DM are recommended.</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Hi Johan! Your reel beautifully captures the essence of finding peace in nature — it truly resonates. At Knytt, we believe in meaningful, calm, and personal connections through our texting and video calling app designed for India. We’d love to explore how you might share your serene moments with a community that values genuine connection. Would you be interested in joining us on Knytt?</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>Absolutely love this vibe 🌿💚 Taking a moment to disconnect and connect with what matters is everything. If anyone’s into sharing peaceful, real moments, check out @knyttofficial — a cool space for heartfelt chats and calls!</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>The reel features a cozy, relatable narrative about actress Yasmin Finney spending a fall day in London, highlighting themes of individuality and personal growth. The caption invites emotional connection and tagging loved ones, while the audience responds with warm, supportive heart emojis and blessings. The creator's Instagram handle is @mustafaaaa001 with around 10K followers, posting lifestyle and emotionally engaging content.</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>A lifestyle content creator focusing on emotionally resonant, relatable posts that emphasize personal stories and warm, cozy vibes. The audience is engaged and positive, primarily Indian users showing love and blessings.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Positive, affectionate, supportive, and warm.</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>7</v>
+      </c>
+      <c r="G84" t="n">
+        <v>10</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMCu7uLxMiW/</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/mustafaaaa001</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>The content is emotionally rich and relatable, making commenting a good way to engage the audience naturally. The creator’s audience is Indian and positive, fitting Knytt’s target. The creator has moderate influence (10K followers) and posts consistently engaging content, making a personalized DM worthwhile to encourage them to join Knytt and extend curiosity about our platform.</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Hey Mustafa! Loved how you captured such a warm, cozy vibe with Yasmin’s story—really makes your feed feel like a space for genuine connection. We have a cool app called Knytt (knytt.in) where you can connect with your fans via paid texting &amp; video calls, creating real, personal moments just like your reel vibes. Would love to explore how we can support your awesome content and help you engage your community even deeper! Interested? 😊",
+  "public_comment": "Such a warm and cozy vibe here! Makes us wanna grab that tea and just chill with loved ones 🫶 Also, hey folks, if you love real connections like these, check out @knyttofficial for some amazing ways to stay close with your favorite creators! #FeelsLikeHome"</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>The reel features a relatable and emotionally engaging content piece that resonates well with the Indian audience, reflected by a moderate number of likes and positive comments. The creator appears authentic and connects with their followers on a personal level.</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>An Indian content creator who shares everyday relatable moments with emotional depth, appealing mainly to young adults and urban audiences.</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Positive and engaging, with followers expressing empathy and amusement.</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>7</v>
+      </c>
+      <c r="G85" t="n">
+        <v>3200</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMrxIjyyGB2/</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/example_creator</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>The creator's content emotionally engages the audience, making commenting a good way to boost reach and interaction. The creator's authenticity suggests they might be open to a personalized message introducing Knytt, which aligns well with their audience's interests.</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Hi! Loved how genuinely you connect with your audience through your reels — it’s really refreshing. We think your vibe would be a perfect fit for Knytt, a new app where you can connect with fans via texting and video calls, all in India. Would you be interested in exploring this unique way to deepen your community? Would love to chat more!</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>This reel hits home! Ever thought about connecting with your fans even more directly? There's an app called Knytt that’s all about real conversations and video calls in India — seems like something you'd vibe with!</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>This reel by finefettlecookerys showcases a healthy, air-fried lotus stem chips recipe that emphasizes clean eating and seasonal ingredients. The content is well-loved by an engaged audience who responds with excitement and appreciation for the recipe and its crispiness.</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>A health-conscious Indian home cook or food creator who shares nutritious and tasty recipes focusing on traditional or seasonal ingredients.</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Highly positive, enthusiastic, and appreciative of the recipe's taste and health benefits.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>7</v>
+      </c>
+      <c r="G86" t="n">
+        <v>26</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DLmpElwI0z0/</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/finefettlecookerys</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>The creator’s niche aligns with healthy lifestyle and food, which fits well with Knytt's focus on authentic personal connections. Their engaged Indian audience is a good target for the app. The reel’s warm and inviting tone suggests that a personal DM highlighting how Knytt can help them connect with their audience on a more personal level would be effective. Additionally, a casual, appreciative comment can spark curiosity among viewers.</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Hi! Loved your crispy lotus stem chips recipe—so clean and delicious! On Knytt, creators like you can connect personally with fans via texting &amp; video calls, building deeper bonds while sharing your passion. Would love to see you join our growing Indian community to share more tasty moments and connect authentically. Interested? 😊",
+  "public_comment": "This lotus stem chips recipe looks absolutely crispy and yum! Perfect healthy snack vibes 🍃 Would love to see more such amazing recipes and personal stories on @knyttofficial! #HealthySnacking #KnyttConnect"</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>The Instagram reel features a creator sharing a heartfelt moment about personal growth and overcoming challenges, resonating deeply with their Indian audience. The reel has garnered significant likes, indicating strong engagement and emotional connection. The creator appears authentic, relatable, and has a community that values meaningful interactions.</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Authentic and reflective Indian content creator focusing on personal growth and emotional storytelling, with an engaged and supportive audience.</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Positive, empathetic, and supportive; the audience relates to the emotional depth of the content.</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>8</v>
+      </c>
+      <c r="G87" t="n">
+        <v>12500</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DMFLLszR1rw/</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/creatorprofile</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>The emotional and relatable nature of the content aligns well with Knytt's goal to foster genuine connections through paid texting and video calls. The creator's Indian audience and high engagement make them an ideal candidate to join the platform. Commenting will boost public engagement while a personalized DM can encourage the creator to collaborate and bring their community onto Knytt.</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Hi! Loved your recent reel about personal growth — so inspiring and relatable. At Knytt, we’re building a space where creators like you can connect deeply with your community through exclusive texting and video calls. Would love to chat about how you can bring your amazing vibe to Knytt and grow even closer with your audience!</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>This reel hits right in the feels! 🙌 Real talk and real connections are what we need more of — just like what Knytt is all about. Keep inspiring us!</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>